<commit_message>
upgraded validation test cases to oed2 format
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\joh\Joh\07 Dev\FM\conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554CA6A3-837B-4C05-A101-277681824515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FD95A-33E6-463B-B1B7-6897BBF91291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -54,9 +54,6 @@
     <t>fm41</t>
   </si>
   <si>
-    <t>A single special condition affecting 2 locations</t>
-  </si>
-  <si>
     <t>fm12</t>
   </si>
   <si>
@@ -102,15 +99,9 @@
     <t>sc12</t>
   </si>
   <si>
-    <t>3 special conditions per layer (7 policies) - original implementation</t>
-  </si>
-  <si>
     <t>File preparation</t>
   </si>
   <si>
-    <t>sc13</t>
-  </si>
-  <si>
     <t>#Locations</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>#Conditions</t>
   </si>
   <si>
-    <t>3 special conditions per layer (7 policies) - different cond numbers per layer</t>
-  </si>
-  <si>
     <t>(A1) Hierarchal sublimits (parent with three children) on one policy - small</t>
   </si>
   <si>
@@ -172,13 +160,25 @@
   </si>
   <si>
     <t>Currently supported</t>
+  </si>
+  <si>
+    <t>A single special condition affecting 3 locations</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>For OED2, duplicates in location removed</t>
+  </si>
+  <si>
+    <t>3 special conditions per layer (7 policies)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +190,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,10 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,38 +566,41 @@
     <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -607,16 +617,16 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -630,21 +640,21 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -656,47 +666,50 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -705,50 +718,53 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>12</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>88</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -756,103 +772,109 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>5</v>
+      <c r="D9" s="3">
+        <v>483</v>
       </c>
       <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
         <v>44</v>
       </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>483</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>16</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -860,51 +882,54 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>2</v>
+      <c r="D13" s="3">
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -913,100 +938,75 @@
         <v>4</v>
       </c>
       <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>497</v>
       </c>
       <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
       <c r="H17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>497</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added original test case for #813
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FD95A-33E6-463B-B1B7-6897BBF91291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4408AE3-C720-478B-AF53-DA655EC1DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>3 special conditions per layer (7 policies)</t>
+  </si>
+  <si>
+    <t>sc13</t>
+  </si>
+  <si>
+    <t>A(5803) Single hierarchy conditions, two policies. one extra condition on one policy</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,7 +566,7 @@
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
@@ -1005,6 +1011,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added expected for sc units
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4408AE3-C720-478B-AF53-DA655EC1DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3177E6-BCCD-4D5D-BDA6-94AE7B42B838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>A(5803) Single hierarchy conditions, two policies. one extra condition on one policy</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +632,7 @@
         <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -655,7 +658,7 @@
         <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -681,7 +684,7 @@
         <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
         <v>44</v>
@@ -710,7 +713,7 @@
         <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -736,7 +739,7 @@
         <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -762,7 +765,7 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
         <v>44</v>
@@ -791,7 +794,7 @@
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
added version of sc13  with 4 locations
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3177E6-BCCD-4D5D-BDA6-94AE7B42B838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42D8CA4-9A76-424C-AEA7-EE16E666040E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -177,10 +177,16 @@
     <t>sc13</t>
   </si>
   <si>
-    <t>A(5803) Single hierarchy conditions, two policies. one extra condition on one policy</t>
-  </si>
-  <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>A(5803) Single hierarchy conditions, two policies. one extra condition on one policy - small</t>
+  </si>
+  <si>
+    <t>A(5803) Single hierarchy conditions, two policies. one extra condition on one policy - big</t>
+  </si>
+  <si>
+    <t>sc14</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +575,7 @@
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
@@ -632,7 +638,7 @@
         <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -658,7 +664,7 @@
         <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -684,7 +690,7 @@
         <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
         <v>44</v>
@@ -713,7 +719,7 @@
         <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -739,7 +745,7 @@
         <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -765,7 +771,7 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
         <v>44</v>
@@ -794,7 +800,7 @@
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
         <v>44</v>
@@ -1022,13 +1028,13 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
@@ -1037,6 +1043,32 @@
         <v>40</v>
       </c>
       <c r="H18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
special conditions expected results
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42D8CA4-9A76-424C-AEA7-EE16E666040E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC233757-9B5E-473C-97DB-DDA796227A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>For OED2, duplicates in location removed</t>
-  </si>
-  <si>
     <t>3 special conditions per layer (7 policies)</t>
   </si>
   <si>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>sc14</t>
+  </si>
+  <si>
+    <t>sc15</t>
+  </si>
+  <si>
+    <t>Single hierarchy conditions One policy. One location with overlapping conditions</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H14" sqref="H14:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +641,7 @@
         <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -664,7 +667,7 @@
         <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -681,7 +684,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -690,10 +693,7 @@
         <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
         <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -771,10 +771,7 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -800,10 +797,7 @@
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -883,9 +877,6 @@
       <c r="H12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -912,9 +903,6 @@
       <c r="H13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -936,10 +924,10 @@
         <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -962,10 +950,10 @@
         <v>32</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -988,10 +976,10 @@
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1014,15 +1002,15 @@
         <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1034,21 +1022,21 @@
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1060,15 +1048,41 @@
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
       </c>
       <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more updates to expected
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC233757-9B5E-473C-97DB-DDA796227A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6438EC21-B0A4-4EAD-B8C9-0B02A1378D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>fm40</t>
-  </si>
-  <si>
-    <t>No conditions, multiple policy layers</t>
   </si>
   <si>
     <t>fm41</t>
@@ -567,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,28 +588,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -623,82 +617,82 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>18</v>
-      </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -707,50 +701,50 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>88</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -759,50 +753,50 @@
         <v>4</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>483</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>483</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -811,50 +805,50 @@
         <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -863,50 +857,50 @@
         <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>105</v>
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -915,102 +909,102 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>497</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>497</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1019,71 +1013,45 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
         <v>38</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test case sc16 for oasislmf issue #1207
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_1207\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6438EC21-B0A4-4EAD-B8C9-0B02A1378D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021A43E-0125-4BCD-B02E-4C778F27B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Single hierarchy conditions One policy. One location with overlapping conditions</t>
+  </si>
+  <si>
+    <t>sc16</t>
+  </si>
+  <si>
+    <t>A sublimit and a restriction on one of two policies</t>
   </si>
 </sst>
 </file>
@@ -242,11 +248,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,29 +566,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.31640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="75.6796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -612,7 +617,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -638,7 +643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -664,7 +669,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -690,7 +695,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -716,7 +721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -726,7 +731,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
@@ -742,7 +747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -752,7 +757,7 @@
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>483</v>
       </c>
       <c r="E8" t="s">
@@ -768,7 +773,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -778,7 +783,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -794,7 +799,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -804,7 +809,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>35</v>
       </c>
       <c r="E10" t="s">
@@ -820,7 +825,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -830,7 +835,7 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
@@ -846,7 +851,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -856,7 +861,7 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>105</v>
       </c>
       <c r="E12" t="s">
@@ -872,7 +877,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -898,7 +903,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -924,7 +929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -950,7 +955,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -976,7 +981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1052,6 +1057,32 @@
       </c>
       <c r="H19" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use Policy CondClass to assess if full filter (exclusion) needs to be used (#1209)
* use Policy CondClass to assess if full filter (exclusion) needs to be used

* added test case sc16 for oasislmf issue #1207

* add fm insurance_condition test case sc16

---------

Co-authored-by: joh <johanna.carter@oasislmf.org>
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_oed2tests\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_1207\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6438EC21-B0A4-4EAD-B8C9-0B02A1378D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021A43E-0125-4BCD-B02E-4C778F27B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Single hierarchy conditions One policy. One location with overlapping conditions</t>
+  </si>
+  <si>
+    <t>sc16</t>
+  </si>
+  <si>
+    <t>A sublimit and a restriction on one of two policies</t>
   </si>
 </sst>
 </file>
@@ -242,11 +248,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,29 +566,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.31640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="75.6796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -612,7 +617,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -638,7 +643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -664,7 +669,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -690,7 +695,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -716,7 +721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -726,7 +731,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
@@ -742,7 +747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -752,7 +757,7 @@
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>483</v>
       </c>
       <c r="E8" t="s">
@@ -768,7 +773,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -778,7 +783,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -794,7 +799,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -804,7 +809,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>35</v>
       </c>
       <c r="E10" t="s">
@@ -820,7 +825,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -830,7 +835,7 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
@@ -846,7 +851,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -856,7 +861,7 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>105</v>
       </c>
       <c r="E12" t="s">
@@ -872,7 +877,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -898,7 +903,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -924,7 +929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -950,7 +955,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -976,7 +981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1052,6 +1057,32 @@
       </c>
       <c r="H19" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for PR #1420
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_1207\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_branch\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021A43E-0125-4BCD-B02E-4C778F27B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AB948F-93AD-4F59-B236-156CD6B4C839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>A sublimit and a restriction on one of two policies</t>
+  </si>
+  <si>
+    <t>sc17</t>
+  </si>
+  <si>
+    <t>Hierarchal conditions. All locations duplicated some with blank cond tag. Tests PR#1420</t>
+  </si>
+  <si>
+    <t>sc18</t>
+  </si>
+  <si>
+    <t>Simple two location version of sc17. Includes duplicate loc 2 with blank cond tag.</t>
+  </si>
+  <si>
+    <t>Simple two location version of sc17. No duplicate loc 2.</t>
+  </si>
+  <si>
+    <t>sc19</t>
   </si>
 </sst>
 </file>
@@ -270,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -416,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,29 +584,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="75.6796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -617,7 +635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -643,7 +661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -669,7 +687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -695,7 +713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -721,7 +739,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -747,7 +765,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -773,7 +791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -799,7 +817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -825,7 +843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -851,7 +869,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -877,7 +895,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -903,7 +921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -929,7 +947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -955,7 +973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -981,7 +999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1007,7 +1025,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1059,7 +1077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1083,6 +1101,84 @@
       </c>
       <c r="H20" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests sc18 and sc19
</commit_message>
<xml_diff>
--- a/validation/insurance_conditions_test_case_list.xlsx
+++ b/validation/insurance_conditions_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_1207\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_branch\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021A43E-0125-4BCD-B02E-4C778F27B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6DE5F-1280-4938-AFF6-89A25C5AD852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5283C321-138E-41C1-9129-B59B6C6B0450}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>Special conditions test cases</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>A sublimit and a restriction on one of two policies</t>
+  </si>
+  <si>
+    <t>sc17</t>
+  </si>
+  <si>
+    <t>Hierarchal conditions. All locations duplicated some with blank cond tag. Tests PR#1420</t>
+  </si>
+  <si>
+    <t>sc18</t>
+  </si>
+  <si>
+    <t>Simple two location version of sc17. Includes duplicate loc 2 with blank cond tag.</t>
+  </si>
+  <si>
+    <t>Simple two location version of sc17. No duplicate loc 2.</t>
+  </si>
+  <si>
+    <t>sc19</t>
   </si>
 </sst>
 </file>
@@ -270,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -416,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,29 +584,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE13B5C-F51E-433D-B41B-794751290FB7}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="75.6796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -617,7 +633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -643,7 +659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -669,7 +685,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -695,7 +711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -721,7 +737,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -747,7 +763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -773,7 +789,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -799,7 +815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -825,7 +841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -851,7 +867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -877,7 +893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -903,7 +919,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -929,7 +945,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -955,7 +971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -981,7 +997,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1007,7 +1023,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1033,7 +1049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1059,7 +1075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1082,6 +1098,84 @@
         <v>36</v>
       </c>
       <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>